<commit_message>
ADD AI's framework resources AND example graphs used for report
</commit_message>
<xml_diff>
--- a/test_images/apples_images/apples_images_mroi/mroi_features.xlsx
+++ b/test_images/apples_images/apples_images_mroi/mroi_features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Desktop\Riccardo Carroccio\CV@TR2\test_images\apples_images\apples_images_mroi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16455F66-4AF6-4548-95D2-D5A281DF1640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E2C87B-070F-446C-94B1-8BBB46D08145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="358" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4665" yWindow="2565" windowWidth="20460" windowHeight="10770" tabRatio="358" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,26 +527,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1146,26 +1126,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2331,26 +2291,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3548,1229 +3488,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5286,558 +4004,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6858,7 +5025,7 @@
   <dimension ref="A1:W100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13280,6 +11447,10 @@
       <c r="G92" s="6" t="s">
         <v>118</v>
       </c>
+      <c r="Q92">
+        <f>AVERAGE(Q2:Q90)</f>
+        <v>6.9397513896693788</v>
+      </c>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F93">

</xml_diff>